<commit_message>
Updated player picks import excel file.
</commit_message>
<xml_diff>
--- a/static/nfl-2022-player-picks.xlsx
+++ b/static/nfl-2022-player-picks.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="111">
   <si>
     <t>Player</t>
   </si>
@@ -345,9 +345,6 @@
   </si>
   <si>
     <t>W</t>
-  </si>
-  <si>
-    <t>TEX</t>
   </si>
 </sst>
 </file>
@@ -2708,7 +2705,7 @@
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3">
         <v>4.5</v>

</xml_diff>